<commit_message>
Generated more Tukey results for CBH Vmax
So as mentioned before, I realized that with the Tukey results rendering some of the significant results from ANOVAs as insignificant, then that frees me up to test certain main effects. Turns out the only new main effect that I can test is Precipitation on CBH Vmax, though. So I re-ran Tukey tests, and turns out this time around it generates timePoint x Vegetation on CBH Vmax for me as well, so I'm guessing that I must have accidentally Tukey results for this interaction before.

So now, I got 1 new main effect (Precipitation) and 1 new interaction (timePoint x Vegetation) for CBH Vmax.

I've annotated groups for timePoint x Vegetation. Now, I'm going to annotate groups for Precip as well.
</commit_message>
<xml_diff>
--- a/Statistical analyses/Tukey posthoc/CBH/Vmax, timePoint x Vegetation.xlsx
+++ b/Statistical analyses/Tukey posthoc/CBH/Vmax, timePoint x Vegetation.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Statistical analyses\Tukey posthoc\CBH\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE82918-422D-472D-83D8-C9CC8B8FA0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="13500" yWindow="3120" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -64,8 +70,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,12 +88,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -117,17 +129,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -174,7 +196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,9 +228,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,6 +280,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,14 +473,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,122 +508,122 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>1.2834</v>
-      </c>
-      <c r="D2">
-        <v>0.001</v>
-      </c>
-      <c r="E2">
-        <v>0.8978</v>
-      </c>
-      <c r="F2">
+      <c r="C2" s="2">
+        <v>1.2834000000000001</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.89780000000000004</v>
+      </c>
+      <c r="F2" s="2">
         <v>1.6691</v>
       </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="G2" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>0.471</v>
-      </c>
-      <c r="D3">
-        <v>0.006999999999999999</v>
-      </c>
-      <c r="E3">
-        <v>0.0854</v>
-      </c>
-      <c r="F3">
-        <v>0.8567</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+      <c r="C3" s="2">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>8.5400000000000004E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.85670000000000002</v>
+      </c>
+      <c r="G3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1.1413</v>
       </c>
-      <c r="D4">
-        <v>0.001</v>
-      </c>
-      <c r="E4">
-        <v>0.7557</v>
-      </c>
-      <c r="F4">
-        <v>1.527</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="D4" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.75570000000000004</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.5269999999999999</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
-        <v>0.4064</v>
-      </c>
-      <c r="D5">
-        <v>0.032</v>
-      </c>
-      <c r="E5">
-        <v>0.0208</v>
-      </c>
-      <c r="F5">
-        <v>0.7921</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+      <c r="C5" s="2">
+        <v>0.40639999999999998</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.79210000000000003</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>1.1751</v>
       </c>
-      <c r="D6">
-        <v>0.001</v>
-      </c>
-      <c r="E6">
-        <v>0.7895</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.78949999999999998</v>
+      </c>
+      <c r="F6" s="2">
         <v>1.5607</v>
       </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -568,68 +631,68 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>0.179</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="D7">
-        <v>0.8021</v>
+        <v>0.80210000000000004</v>
       </c>
       <c r="E7">
-        <v>-0.2066</v>
+        <v>-0.20660000000000001</v>
       </c>
       <c r="F7">
-        <v>0.5647</v>
+        <v>0.56469999999999998</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8">
-        <v>0.8663</v>
-      </c>
-      <c r="D8">
-        <v>0.001</v>
-      </c>
-      <c r="E8">
-        <v>0.4807</v>
-      </c>
-      <c r="F8">
+      <c r="C8" s="2">
+        <v>0.86629999999999996</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.48070000000000002</v>
+      </c>
+      <c r="F8" s="2">
         <v>1.252</v>
       </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+      <c r="G8" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
-        <v>-0.8124</v>
-      </c>
-      <c r="D9">
-        <v>0.001</v>
-      </c>
-      <c r="E9">
+      <c r="C9" s="2">
+        <v>-0.81240000000000001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E9" s="2">
         <v>-1.198</v>
       </c>
-      <c r="F9">
-        <v>-0.4268</v>
-      </c>
-      <c r="G9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9" s="2">
+        <v>-0.42680000000000001</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -643,39 +706,39 @@
         <v>0.9</v>
       </c>
       <c r="E10">
-        <v>-0.5276999999999999</v>
+        <v>-0.52769999999999995</v>
       </c>
       <c r="F10">
-        <v>0.2435</v>
+        <v>0.24349999999999999</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>-0.877</v>
       </c>
-      <c r="D11">
-        <v>0.001</v>
-      </c>
-      <c r="E11">
-        <v>-1.2626</v>
-      </c>
-      <c r="F11">
+      <c r="D11" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>-1.2625999999999999</v>
+      </c>
+      <c r="F11" s="2">
         <v>-0.4914</v>
       </c>
-      <c r="G11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="G11" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -689,85 +752,85 @@
         <v>0.9</v>
       </c>
       <c r="E12">
-        <v>-0.494</v>
+        <v>-0.49399999999999999</v>
       </c>
       <c r="F12">
-        <v>0.2773</v>
+        <v>0.27729999999999999</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>-1.1044</v>
       </c>
-      <c r="D13">
-        <v>0.001</v>
-      </c>
-      <c r="E13">
+      <c r="D13" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E13" s="2">
         <v>-1.49</v>
       </c>
-      <c r="F13">
-        <v>-0.7188</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
+      <c r="F13" s="2">
+        <v>-0.71879999999999999</v>
+      </c>
+      <c r="G13" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
-        <v>-0.4171</v>
-      </c>
-      <c r="D14">
-        <v>0.0252</v>
-      </c>
-      <c r="E14">
-        <v>-0.8027</v>
-      </c>
-      <c r="F14">
-        <v>-0.0315</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
+      <c r="C14" s="2">
+        <v>-0.41710000000000003</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2.52E-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-0.80269999999999997</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-3.15E-2</v>
+      </c>
+      <c r="G14" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15">
-        <v>0.6703</v>
-      </c>
-      <c r="D15">
-        <v>0.001</v>
-      </c>
-      <c r="E15">
-        <v>0.2847</v>
-      </c>
-      <c r="F15">
-        <v>1.0559</v>
-      </c>
-      <c r="G15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="C15" s="2">
+        <v>0.67030000000000001</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.28470000000000001</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.0559000000000001</v>
+      </c>
+      <c r="G15" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -775,45 +838,45 @@
         <v>11</v>
       </c>
       <c r="C16">
-        <v>-0.0646</v>
+        <v>-6.4600000000000005E-2</v>
       </c>
       <c r="D16">
         <v>0.9</v>
       </c>
       <c r="E16">
-        <v>-0.4502</v>
+        <v>-0.45019999999999999</v>
       </c>
       <c r="F16">
-        <v>0.321</v>
+        <v>0.32100000000000001</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17">
-        <v>0.7040000000000001</v>
-      </c>
-      <c r="D17">
-        <v>0.001</v>
-      </c>
-      <c r="E17">
-        <v>0.3184</v>
-      </c>
-      <c r="F17">
-        <v>1.0897</v>
-      </c>
-      <c r="G17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="C17" s="2">
+        <v>0.70400000000000007</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.31840000000000002</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.0896999999999999</v>
+      </c>
+      <c r="G17" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -821,68 +884,68 @@
         <v>13</v>
       </c>
       <c r="C18">
-        <v>-0.292</v>
+        <v>-0.29199999999999998</v>
       </c>
       <c r="D18">
-        <v>0.2694</v>
+        <v>0.26939999999999997</v>
       </c>
       <c r="E18">
-        <v>-0.6776</v>
+        <v>-0.67759999999999998</v>
       </c>
       <c r="F18">
-        <v>0.0936</v>
+        <v>9.3600000000000003E-2</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C19">
-        <v>0.3953</v>
-      </c>
-      <c r="D19">
-        <v>0.0408</v>
-      </c>
-      <c r="E19">
-        <v>0.0097</v>
-      </c>
-      <c r="F19">
-        <v>0.7809</v>
-      </c>
-      <c r="G19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
+      <c r="C19" s="2">
+        <v>0.39529999999999998</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.78090000000000004</v>
+      </c>
+      <c r="G19" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>-0.7349</v>
       </c>
-      <c r="D20">
-        <v>0.001</v>
-      </c>
-      <c r="E20">
-        <v>-1.1205</v>
-      </c>
-      <c r="F20">
+      <c r="D20" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E20" s="2">
+        <v>-1.1205000000000001</v>
+      </c>
+      <c r="F20" s="2">
         <v>-0.3493</v>
       </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="G20" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -890,13 +953,13 @@
         <v>12</v>
       </c>
       <c r="C21">
-        <v>0.0337</v>
+        <v>3.3700000000000001E-2</v>
       </c>
       <c r="D21">
         <v>0.9</v>
       </c>
       <c r="E21">
-        <v>-0.3519</v>
+        <v>-0.35189999999999999</v>
       </c>
       <c r="F21">
         <v>0.4194</v>
@@ -905,30 +968,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C22">
-        <v>-0.9623</v>
-      </c>
-      <c r="D22">
-        <v>0.001</v>
-      </c>
-      <c r="E22">
-        <v>-1.3479</v>
-      </c>
-      <c r="F22">
-        <v>-0.5767</v>
-      </c>
-      <c r="G22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="C22" s="2">
+        <v>-0.96230000000000004</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>-1.3479000000000001</v>
+      </c>
+      <c r="F22" s="2">
+        <v>-0.57669999999999999</v>
+      </c>
+      <c r="G22" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -936,13 +999,13 @@
         <v>14</v>
       </c>
       <c r="C23">
-        <v>-0.275</v>
+        <v>-0.27500000000000002</v>
       </c>
       <c r="D23">
-        <v>0.3421</v>
+        <v>0.34210000000000002</v>
       </c>
       <c r="E23">
-        <v>-0.6606</v>
+        <v>-0.66059999999999997</v>
       </c>
       <c r="F23">
         <v>0.1106</v>
@@ -951,30 +1014,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C24">
-        <v>0.7685999999999999</v>
-      </c>
-      <c r="D24">
-        <v>0.001</v>
-      </c>
-      <c r="E24">
-        <v>0.383</v>
-      </c>
-      <c r="F24">
-        <v>1.1543</v>
-      </c>
-      <c r="G24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="C24" s="2">
+        <v>0.76859999999999995</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.1543000000000001</v>
+      </c>
+      <c r="G24" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -982,68 +1045,68 @@
         <v>13</v>
       </c>
       <c r="C25">
-        <v>-0.2274</v>
+        <v>-0.22739999999999999</v>
       </c>
       <c r="D25">
-        <v>0.5745</v>
+        <v>0.57450000000000001</v>
       </c>
       <c r="E25">
-        <v>-0.613</v>
+        <v>-0.61299999999999999</v>
       </c>
       <c r="F25">
-        <v>0.1582</v>
+        <v>0.15820000000000001</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C26">
-        <v>0.4599</v>
-      </c>
-      <c r="D26">
-        <v>0.0092</v>
-      </c>
-      <c r="E26">
-        <v>0.0743</v>
-      </c>
-      <c r="F26">
-        <v>0.8455</v>
-      </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
+      <c r="C26" s="2">
+        <v>0.45989999999999998</v>
+      </c>
+      <c r="D26" s="2">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="E26" s="2">
+        <v>7.4300000000000005E-2</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.84550000000000003</v>
+      </c>
+      <c r="G26" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>-0.996</v>
       </c>
-      <c r="D27">
-        <v>0.001</v>
-      </c>
-      <c r="E27">
-        <v>-1.3816</v>
-      </c>
-      <c r="F27">
-        <v>-0.6104000000000001</v>
-      </c>
-      <c r="G27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="D27" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E27" s="2">
+        <v>-1.3815999999999999</v>
+      </c>
+      <c r="F27" s="2">
+        <v>-0.61040000000000005</v>
+      </c>
+      <c r="G27" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1051,41 +1114,41 @@
         <v>14</v>
       </c>
       <c r="C28">
-        <v>-0.3087</v>
+        <v>-0.30869999999999997</v>
       </c>
       <c r="D28">
-        <v>0.2083</v>
+        <v>0.20830000000000001</v>
       </c>
       <c r="E28">
-        <v>-0.6944</v>
+        <v>-0.69440000000000002</v>
       </c>
       <c r="F28">
-        <v>0.0769</v>
+        <v>7.6899999999999996E-2</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C29">
-        <v>0.6873</v>
-      </c>
-      <c r="D29">
-        <v>0.001</v>
-      </c>
-      <c r="E29">
-        <v>0.3017</v>
-      </c>
-      <c r="F29">
+      <c r="C29" s="2">
+        <v>0.68730000000000002</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.30170000000000002</v>
+      </c>
+      <c r="F29" s="2">
         <v>1.0729</v>
       </c>
-      <c r="G29" t="b">
+      <c r="G29" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a function to allow me to export raw Tukey results
This is a convenience function intended for when I decide to run Tukey's on treatments and interactions that weren't tested for when I run them using the first Tukey function in the Tukey.py script.

When I ran this whole script again, I accidentally created some new files, including new timePoint x Vegetation raw Tukey results. I am not going through and manually annotating this, again. I'm too lazy for that.
</commit_message>
<xml_diff>
--- a/Statistical analyses/Tukey posthoc/CBH/Vmax, timePoint x Vegetation.xlsx
+++ b/Statistical analyses/Tukey posthoc/CBH/Vmax, timePoint x Vegetation.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Statistical analyses\Tukey posthoc\CBH\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE82918-422D-472D-83D8-C9CC8B8FA0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="3120" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -70,8 +64,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,18 +82,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -129,27 +117,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -196,7 +174,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,27 +206,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,24 +240,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -473,19 +415,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,122 +445,122 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2">
-        <v>1.2834000000000001</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.89780000000000004</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="C2">
+        <v>1.2834</v>
+      </c>
+      <c r="D2">
+        <v>0.001</v>
+      </c>
+      <c r="E2">
+        <v>0.8978</v>
+      </c>
+      <c r="F2">
         <v>1.6691</v>
       </c>
-      <c r="G2" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.47099999999999997</v>
-      </c>
-      <c r="D3" s="2">
-        <v>6.9999999999999993E-3</v>
-      </c>
-      <c r="E3" s="2">
-        <v>8.5400000000000004E-2</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.85670000000000002</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="C3">
+        <v>0.471</v>
+      </c>
+      <c r="D3">
+        <v>0.006999999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.0854</v>
+      </c>
+      <c r="F3">
+        <v>0.8567</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>1.1413</v>
       </c>
-      <c r="D4" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.75570000000000004</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.5269999999999999</v>
-      </c>
-      <c r="G4" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="D4">
+        <v>0.001</v>
+      </c>
+      <c r="E4">
+        <v>0.7557</v>
+      </c>
+      <c r="F4">
+        <v>1.527</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2">
-        <v>0.40639999999999998</v>
-      </c>
-      <c r="D5" s="2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>2.0799999999999999E-2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.79210000000000003</v>
-      </c>
-      <c r="G5" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="C5">
+        <v>0.4064</v>
+      </c>
+      <c r="D5">
+        <v>0.032</v>
+      </c>
+      <c r="E5">
+        <v>0.0208</v>
+      </c>
+      <c r="F5">
+        <v>0.7921</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>1.1751</v>
       </c>
-      <c r="D6" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.78949999999999998</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="D6">
+        <v>0.001</v>
+      </c>
+      <c r="E6">
+        <v>0.7895</v>
+      </c>
+      <c r="F6">
         <v>1.5607</v>
       </c>
-      <c r="G6" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -631,68 +568,68 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>0.17899999999999999</v>
+        <v>0.179</v>
       </c>
       <c r="D7">
-        <v>0.80210000000000004</v>
+        <v>0.8021</v>
       </c>
       <c r="E7">
-        <v>-0.20660000000000001</v>
+        <v>-0.2066</v>
       </c>
       <c r="F7">
-        <v>0.56469999999999998</v>
+        <v>0.5647</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2">
-        <v>0.86629999999999996</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.48070000000000002</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="C8">
+        <v>0.8663</v>
+      </c>
+      <c r="D8">
+        <v>0.001</v>
+      </c>
+      <c r="E8">
+        <v>0.4807</v>
+      </c>
+      <c r="F8">
         <v>1.252</v>
       </c>
-      <c r="G8" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2">
-        <v>-0.81240000000000001</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="C9">
+        <v>-0.8124</v>
+      </c>
+      <c r="D9">
+        <v>0.001</v>
+      </c>
+      <c r="E9">
         <v>-1.198</v>
       </c>
-      <c r="F9" s="2">
-        <v>-0.42680000000000001</v>
-      </c>
-      <c r="G9" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>-0.4268</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -706,39 +643,39 @@
         <v>0.9</v>
       </c>
       <c r="E10">
-        <v>-0.52769999999999995</v>
+        <v>-0.5276999999999999</v>
       </c>
       <c r="F10">
-        <v>0.24349999999999999</v>
+        <v>0.2435</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>-0.877</v>
       </c>
-      <c r="D11" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E11" s="2">
-        <v>-1.2625999999999999</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="D11">
+        <v>0.001</v>
+      </c>
+      <c r="E11">
+        <v>-1.2626</v>
+      </c>
+      <c r="F11">
         <v>-0.4914</v>
       </c>
-      <c r="G11" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -752,85 +689,85 @@
         <v>0.9</v>
       </c>
       <c r="E12">
-        <v>-0.49399999999999999</v>
+        <v>-0.494</v>
       </c>
       <c r="F12">
-        <v>0.27729999999999999</v>
+        <v>0.2773</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>-1.1044</v>
       </c>
-      <c r="D13" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="D13">
+        <v>0.001</v>
+      </c>
+      <c r="E13">
         <v>-1.49</v>
       </c>
-      <c r="F13" s="2">
-        <v>-0.71879999999999999</v>
-      </c>
-      <c r="G13" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="F13">
+        <v>-0.7188</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2">
-        <v>-0.41710000000000003</v>
-      </c>
-      <c r="D14" s="2">
-        <v>2.52E-2</v>
-      </c>
-      <c r="E14" s="2">
-        <v>-0.80269999999999997</v>
-      </c>
-      <c r="F14" s="2">
-        <v>-3.15E-2</v>
-      </c>
-      <c r="G14" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="C14">
+        <v>-0.4171</v>
+      </c>
+      <c r="D14">
+        <v>0.0252</v>
+      </c>
+      <c r="E14">
+        <v>-0.8027</v>
+      </c>
+      <c r="F14">
+        <v>-0.0315</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="2">
-        <v>0.67030000000000001</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.28470000000000001</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1.0559000000000001</v>
-      </c>
-      <c r="G15" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>0.6703</v>
+      </c>
+      <c r="D15">
+        <v>0.001</v>
+      </c>
+      <c r="E15">
+        <v>0.2847</v>
+      </c>
+      <c r="F15">
+        <v>1.0559</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -838,45 +775,45 @@
         <v>11</v>
       </c>
       <c r="C16">
-        <v>-6.4600000000000005E-2</v>
+        <v>-0.0646</v>
       </c>
       <c r="D16">
         <v>0.9</v>
       </c>
       <c r="E16">
-        <v>-0.45019999999999999</v>
+        <v>-0.4502</v>
       </c>
       <c r="F16">
-        <v>0.32100000000000001</v>
+        <v>0.321</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="2">
-        <v>0.70400000000000007</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.31840000000000002</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1.0896999999999999</v>
-      </c>
-      <c r="G17" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>0.7040000000000001</v>
+      </c>
+      <c r="D17">
+        <v>0.001</v>
+      </c>
+      <c r="E17">
+        <v>0.3184</v>
+      </c>
+      <c r="F17">
+        <v>1.0897</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -884,68 +821,68 @@
         <v>13</v>
       </c>
       <c r="C18">
-        <v>-0.29199999999999998</v>
+        <v>-0.292</v>
       </c>
       <c r="D18">
-        <v>0.26939999999999997</v>
+        <v>0.2694</v>
       </c>
       <c r="E18">
-        <v>-0.67759999999999998</v>
+        <v>-0.6776</v>
       </c>
       <c r="F18">
-        <v>9.3600000000000003E-2</v>
+        <v>0.0936</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="2">
-        <v>0.39529999999999998</v>
-      </c>
-      <c r="D19" s="2">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="E19" s="2">
-        <v>9.7000000000000003E-3</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0.78090000000000004</v>
-      </c>
-      <c r="G19" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="C19">
+        <v>0.3953</v>
+      </c>
+      <c r="D19">
+        <v>0.0408</v>
+      </c>
+      <c r="E19">
+        <v>0.0097</v>
+      </c>
+      <c r="F19">
+        <v>0.7809</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>-0.7349</v>
       </c>
-      <c r="D20" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E20" s="2">
-        <v>-1.1205000000000001</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="D20">
+        <v>0.001</v>
+      </c>
+      <c r="E20">
+        <v>-1.1205</v>
+      </c>
+      <c r="F20">
         <v>-0.3493</v>
       </c>
-      <c r="G20" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -953,13 +890,13 @@
         <v>12</v>
       </c>
       <c r="C21">
-        <v>3.3700000000000001E-2</v>
+        <v>0.0337</v>
       </c>
       <c r="D21">
         <v>0.9</v>
       </c>
       <c r="E21">
-        <v>-0.35189999999999999</v>
+        <v>-0.3519</v>
       </c>
       <c r="F21">
         <v>0.4194</v>
@@ -968,30 +905,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="2">
-        <v>-0.96230000000000004</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E22" s="2">
-        <v>-1.3479000000000001</v>
-      </c>
-      <c r="F22" s="2">
-        <v>-0.57669999999999999</v>
-      </c>
-      <c r="G22" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>-0.9623</v>
+      </c>
+      <c r="D22">
+        <v>0.001</v>
+      </c>
+      <c r="E22">
+        <v>-1.3479</v>
+      </c>
+      <c r="F22">
+        <v>-0.5767</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -999,13 +936,13 @@
         <v>14</v>
       </c>
       <c r="C23">
-        <v>-0.27500000000000002</v>
+        <v>-0.275</v>
       </c>
       <c r="D23">
-        <v>0.34210000000000002</v>
+        <v>0.3421</v>
       </c>
       <c r="E23">
-        <v>-0.66059999999999997</v>
+        <v>-0.6606</v>
       </c>
       <c r="F23">
         <v>0.1106</v>
@@ -1014,30 +951,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="2">
-        <v>0.76859999999999995</v>
-      </c>
-      <c r="D24" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="F24" s="2">
-        <v>1.1543000000000001</v>
-      </c>
-      <c r="G24" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>0.7685999999999999</v>
+      </c>
+      <c r="D24">
+        <v>0.001</v>
+      </c>
+      <c r="E24">
+        <v>0.383</v>
+      </c>
+      <c r="F24">
+        <v>1.1543</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1045,68 +982,68 @@
         <v>13</v>
       </c>
       <c r="C25">
-        <v>-0.22739999999999999</v>
+        <v>-0.2274</v>
       </c>
       <c r="D25">
-        <v>0.57450000000000001</v>
+        <v>0.5745</v>
       </c>
       <c r="E25">
-        <v>-0.61299999999999999</v>
+        <v>-0.613</v>
       </c>
       <c r="F25">
-        <v>0.15820000000000001</v>
+        <v>0.1582</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="2">
-        <v>0.45989999999999998</v>
-      </c>
-      <c r="D26" s="2">
-        <v>9.1999999999999998E-3</v>
-      </c>
-      <c r="E26" s="2">
-        <v>7.4300000000000005E-2</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0.84550000000000003</v>
-      </c>
-      <c r="G26" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="C26">
+        <v>0.4599</v>
+      </c>
+      <c r="D26">
+        <v>0.0092</v>
+      </c>
+      <c r="E26">
+        <v>0.0743</v>
+      </c>
+      <c r="F26">
+        <v>0.8455</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>-0.996</v>
       </c>
-      <c r="D27" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E27" s="2">
-        <v>-1.3815999999999999</v>
-      </c>
-      <c r="F27" s="2">
-        <v>-0.61040000000000005</v>
-      </c>
-      <c r="G27" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>0.001</v>
+      </c>
+      <c r="E27">
+        <v>-1.3816</v>
+      </c>
+      <c r="F27">
+        <v>-0.6104000000000001</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1114,41 +1051,41 @@
         <v>14</v>
       </c>
       <c r="C28">
-        <v>-0.30869999999999997</v>
+        <v>-0.3087</v>
       </c>
       <c r="D28">
-        <v>0.20830000000000001</v>
+        <v>0.2083</v>
       </c>
       <c r="E28">
-        <v>-0.69440000000000002</v>
+        <v>-0.6944</v>
       </c>
       <c r="F28">
-        <v>7.6899999999999996E-2</v>
+        <v>0.0769</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="2">
-        <v>0.68730000000000002</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0.30170000000000002</v>
-      </c>
-      <c r="F29" s="2">
+      <c r="C29">
+        <v>0.6873</v>
+      </c>
+      <c r="D29">
+        <v>0.001</v>
+      </c>
+      <c r="E29">
+        <v>0.3017</v>
+      </c>
+      <c r="F29">
         <v>1.0729</v>
       </c>
-      <c r="G29" s="2" t="b">
+      <c r="G29" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>